<commit_message>
add time for teaching
</commit_message>
<xml_diff>
--- a/react-learning.xlsx
+++ b/react-learning.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\django\Desktop\New folder\react-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{560BDA72-8218-4D0A-8533-77EDD2DBA7B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D04469-DEE3-4F17-912C-2A331EB0E661}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="2790" windowWidth="21600" windowHeight="11505" activeTab="1" xr2:uid="{15C9A635-85BB-401C-9C92-3E169DE782F8}"/>
+    <workbookView xWindow="2565" yWindow="2790" windowWidth="21600" windowHeight="11505" xr2:uid="{15C9A635-85BB-401C-9C92-3E169DE782F8}"/>
   </bookViews>
   <sheets>
     <sheet name="به روز رسانی " sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="135">
   <si>
     <t xml:space="preserve">عنوان </t>
   </si>
@@ -158,9 +158,6 @@
   </si>
   <si>
     <t xml:space="preserve">css animation in react </t>
-  </si>
-  <si>
-    <t>UDEMY – REACT – THE COMPLETE GUIDE (INCL HOOKS, REACT ROUTER, REDUX) 2021-12</t>
   </si>
   <si>
     <t>EPIC REACT – GET REALLY GOOD AT REACT | EPIC REACT PRO BY KENT C. DODDS 2021-11</t>
@@ -336,12 +333,6 @@
   </si>
   <si>
     <t xml:space="preserve">کم - متوسط </t>
-  </si>
-  <si>
-    <t>The Complete JavaScript Course 2020 From Zero to Expert</t>
-  </si>
-  <si>
-    <t xml:space="preserve">زمان </t>
   </si>
   <si>
     <t xml:space="preserve">با توجه به مهارت استعداد و میزان آشنایی قبلی 
@@ -391,9 +382,6 @@
 زمان آموزش فرد به فرد متفاووته و نیازه تا مفاهیم جا بیافته 
 تخمینی میشه گفت با روزی 4 ساعت برای این مرحله بین 3 - 6 ماه 
 زمان لازمه که با توجه به مهارت فرد و میزان یاد گیری این  می تونه زمان کمتر یا حتی بیشتر بشه </t>
-  </si>
-  <si>
-    <t xml:space="preserve">زمان بندی </t>
   </si>
   <si>
     <t xml:space="preserve">این مرحله بالا بردن دانش و مهارته 
@@ -432,11 +420,60 @@
     <t xml:space="preserve">نیاز به سئو تو اپ های تک صفحه ای حس میشه </t>
   </si>
   <si>
+    <t xml:space="preserve">فایل اکسل از این طریق به روز رسانی خواهد شد </t>
+  </si>
+  <si>
+    <t xml:space="preserve">زمان خود آموز </t>
+  </si>
+  <si>
+    <t>زمان آموزش (خود آموز)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">زمان تدریس </t>
+  </si>
+  <si>
+    <t xml:space="preserve">دوره های آموزشی مقدماتی ری اکت معمولا
+بین 20-25 ساعت کلاس حضوری بر گزار می کنند 
+که این  نسبت به محتوای آموزش می تواند متغیر باشد </t>
+  </si>
+  <si>
+    <t xml:space="preserve">آموزش es6  و پیشنیاز های ری اکت می تواند در کلاس 
+طی 1 الی 2 جلسه  نهایتا 4 ساعت انجام پذیرد 
+اما دوره  آموزش کامل جاوا اسکریپت  حدودا  25 ساعت کلاس نیاز دارد حداقل </t>
+  </si>
+  <si>
+    <t>زمان بندی (خود آموز)</t>
+  </si>
+  <si>
+    <t>زمان بندی (آموزش)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">در صورت پر محتوا بودن دوره مقدماتی  بسیاری از سر فصل ها می تواند آنجا 
+پوشش داده شود و نیازی به این دوره نباشد .
+اما اگر محتوای این بخش را مجزا بخواهید آموزش دهید به حدود 20-25 ساعت کلاس 
+نیاز است و البته حدود 10-12 ساعت هم کلاس رفع اشکال 
+باز محتوای دوره و سطح دانشجویان از عوامل تاثیر گذار در این بخش می باشند </t>
+  </si>
+  <si>
+    <t>زمان بندی (آموزشی)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">دوره ای در این سطح  موجود نمی باشد و ظاهرا ترجیح بر خود آموز 
+پیشرفتن است 
+با این حال دوره موجود در این سطح 27 ساعت است که می توان گفت آموزش این دوره به حدود 
+30-35 ساعت  نیاز دارد </t>
+  </si>
+  <si>
     <t>FRONTEND MASTERS – INTERMEDIATE REACT, V2 2019-6 by BRIAN HOLT  
-Udemy – Next.js &amp; React – The Complete Guide (incl. Two Paths!) 2021-12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">فایل اکسل از این طریق به روز رسانی خواهد شد </t>
+Udemy – Next.js &amp; React – The Complete Guide (incl. Two Paths!) 2021-12 By MAXIMILIAN SHWARTZMULLER</t>
+  </si>
+  <si>
+    <t>UDEMY – REACT – THE COMPLETE GUIDE (INCL HOOKS, REACT ROUTER, REDUX) 2021-12 
+By MAXIMILIAN SHWARTZMULLER</t>
+  </si>
+  <si>
+    <t>The Complete JavaScript Course 2020 From Zero to Expert 
+By Jonas</t>
   </si>
 </sst>
 </file>
@@ -679,7 +716,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -690,9 +727,6 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -731,9 +765,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -760,6 +791,15 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1082,10 +1122,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A3872D-1D8C-48BC-A485-142E9E20FE81}">
-  <dimension ref="B1:C2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1094,13 +1134,17 @@
     <col min="3" max="3" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:3" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="22" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>126</v>
+    <row r="1" spans="1:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="61.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="20" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1113,163 +1157,170 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="B1:G13"/>
+  <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="7" customWidth="1"/>
-    <col min="2" max="2" width="30.140625" style="8" customWidth="1"/>
-    <col min="3" max="3" width="40.7109375" style="8" customWidth="1"/>
-    <col min="4" max="4" width="29.85546875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="30.140625" style="7" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="7" customWidth="1"/>
+    <col min="4" max="4" width="29.85546875" style="7" customWidth="1"/>
     <col min="6" max="6" width="75.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="34" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="40.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="6" t="s">
+    <row r="1" spans="2:8" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="7" t="s">
+      <c r="G1" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="116.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="17" t="s">
+        <v>95</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>134</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="7" t="s">
+      <c r="D3" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C4" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="F8" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>94</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="7" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="7" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="F8" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="7" t="s">
-        <v>93</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="7"/>
-    </row>
-    <row r="13" spans="2:7" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="7"/>
+    </row>
+    <row r="12" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="6"/>
+    </row>
+    <row r="13" spans="2:8" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -1283,421 +1334,428 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="B1:G36"/>
+  <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="36" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="47.5703125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="57.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="47.5703125" style="9" customWidth="1"/>
+    <col min="3" max="3" width="57.7109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5703125" style="6" customWidth="1"/>
     <col min="6" max="6" width="78.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="54.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="9" t="s">
+    <row r="1" spans="2:8" ht="54.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" ht="84" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+      <c r="G1" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="102.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="10" t="s">
+      <c r="D2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="22" t="s">
+        <v>111</v>
+      </c>
+      <c r="H2" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="D4" s="7" t="s">
+    <row r="9" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="5" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="7" t="s">
+    <row r="10" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="7" t="s">
+    <row r="11" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="D7" s="7" t="s">
+    <row r="12" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="C9" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="D12" s="7" t="s">
+    <row r="26" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B26" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="16" spans="2:7" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C18" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="C20" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C22" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="C23" s="11" t="s">
+    <row r="27" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="28" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="11" t="s">
+      <c r="D28" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="30" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B30" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="D24" s="7" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="25" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="26" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="11" t="s">
+      <c r="D30" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="31" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B31" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="D26" s="7" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="28" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C29" s="11" t="s">
+      <c r="D31" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="32" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="33" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B33" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B30" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="C33" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D34" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B35" s="10" t="s">
+      <c r="C35" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="D35" s="7" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="36" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="7" t="s">
-        <v>83</v>
+      <c r="D36" s="6" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -1711,114 +1769,121 @@
   <sheetPr>
     <tabColor rgb="FF7030A0"/>
   </sheetPr>
-  <dimension ref="B1:G9"/>
+  <dimension ref="B1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="63.42578125" style="14" customWidth="1"/>
-    <col min="3" max="3" width="42.28515625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="25.28515625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="63.42578125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="42.28515625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" style="7" customWidth="1"/>
     <col min="6" max="6" width="86" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="67.28515625" customWidth="1"/>
+    <col min="8" max="8" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="12" t="s">
+    <row r="1" spans="2:8" ht="54" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="11" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="25" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="2" spans="2:7" ht="99.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="13" t="s">
+      <c r="G1" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="126.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" s="26" t="s">
+        <v>132</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>112</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="F2" s="28" t="s">
-        <v>125</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="13" t="s">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="13" t="s">
+      <c r="C4" s="6" t="s">
+        <v>120</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="13" t="s">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="13" t="s">
+      <c r="D6" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="13" t="s">
+      <c r="D7" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="13" t="s">
+      <c r="D8" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="7" t="s">
-        <v>82</v>
+    </row>
+    <row r="9" spans="2:8" ht="27" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="12" t="s">
+        <v>80</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -1831,118 +1896,125 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="B1:G9"/>
+  <dimension ref="B1:H9"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" customHeight="1" thickTop="1" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="45.7109375" style="17" customWidth="1"/>
-    <col min="3" max="3" width="63.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29" style="16" customWidth="1"/>
+    <col min="2" max="2" width="45.7109375" style="16" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29" style="15" customWidth="1"/>
     <col min="6" max="6" width="103.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="45.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="15" t="s">
+    <row r="1" spans="2:8" ht="62.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="14" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" ht="120.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="15" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="G2" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H2" s="24" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="16" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="2" spans="2:7" ht="120.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="17" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="F2" s="27" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="17" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>118</v>
+      <c r="D8" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" ht="26.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>